<commit_message>
Added doc pertaining proofreading
Former-commit-id: 7cd93cb73faf14d375219033ea08d7f15da114f0
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Vid_1 Unclassified.xlsx
+++ b/3 Beginner Videos/Vid_1 Unclassified.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="908" documentId="11_F25DC773A252ABDACC1048EAE15952625BDE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{93FC0CBE-3BDA-4C7F-A20D-C3D01C039B22}"/>
   <bookViews>
-    <workbookView xWindow="13035" yWindow="10920" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24630" yWindow="6765" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1242,8 +1242,8 @@
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>